<commit_message>
Combined extract usage, set supplier and set choice id functions
</commit_message>
<xml_diff>
--- a/10.15.20 - G.xlsx
+++ b/10.15.20 - G.xlsx
@@ -554,13 +554,21 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -578,7 +586,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>6% 281.0</t>
+          <t>17342</t>
         </is>
       </c>
     </row>

</xml_diff>